<commit_message>
updated to reflect 117 total iterations
</commit_message>
<xml_diff>
--- a/data/scenario_table_text.xlsx
+++ b/data/scenario_table_text.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahkoenker/Dropbox/R Directory/Quantification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0FD19A7-5541-214D-8E7D-0F80BE66EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7319CA1-7D74-8040-8BA1-48B6885146D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{D175AB0F-402B-D841-A3E2-CFF385259FBB}"/>
+    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D175AB0F-402B-D841-A3E2-CFF385259FBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pop times" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Scenario</t>
   </si>
@@ -70,18 +72,12 @@
     <t>2021-2035 at 6% of the population</t>
   </si>
   <si>
-    <t>2022-2032 varying from 1-20% of the population</t>
-  </si>
-  <si>
     <t>3. “Mass plus continuous”</t>
   </si>
   <si>
     <t>2020-2035 at 6% of the population</t>
   </si>
   <si>
-    <t>Only in years between campaigns, varying from 1-20% of the population</t>
-  </si>
-  <si>
     <t>4. “Varying 3-year mass”</t>
   </si>
   <si>
@@ -92,6 +88,33 @@
   </si>
   <si>
     <t>In 2022, 2024, 2026, 2028, 2030, 2032, 2034 varying from population / 1.0-2.0</t>
+  </si>
+  <si>
+    <t>2022-2032 varying from 1-40% of the population</t>
+  </si>
+  <si>
+    <t>Only in years between campaigns, varying from 1-40% of the population</t>
+  </si>
+  <si>
+    <t>2020-2035, varying from population x 5% to population x 7%</t>
+  </si>
+  <si>
+    <t>2021-2035 using population x 6%</t>
+  </si>
+  <si>
+    <t>2020-2035 using population x 6%</t>
+  </si>
+  <si>
+    <t>Number of different runs per scenario</t>
+  </si>
+  <si>
+    <t>Total iterations</t>
+  </si>
+  <si>
+    <t>Only in years between campaigns, varying the CD quantifer from population x 0% to population x 40%</t>
+  </si>
+  <si>
+    <t>2022-2032 varying the CD quantifer from population x 0% to population x 50%</t>
   </si>
 </sst>
 </file>
@@ -142,12 +165,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -466,13 +492,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DCD770-2C0F-7B4E-8D42-EBDED73D7214}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -500,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -511,49 +543,181 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="136" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="187" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53775954-0455-D446-9A64-3756E2CFD60A}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E2:E6)</f>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update number of iterations
</commit_message>
<xml_diff>
--- a/data/scenario_table_text.xlsx
+++ b/data/scenario_table_text.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahkoenker/Dropbox/R Directory/Quantification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7319CA1-7D74-8040-8BA1-48B6885146D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDF94B5-AB8D-DD4F-A36D-E89C01183B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D175AB0F-402B-D841-A3E2-CFF385259FBB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Scenario</t>
   </si>
@@ -105,16 +105,22 @@
     <t>2020-2035 using population x 6%</t>
   </si>
   <si>
-    <t>Number of different runs per scenario</t>
-  </si>
-  <si>
     <t>Total iterations</t>
   </si>
   <si>
-    <t>Only in years between campaigns, varying the CD quantifer from population x 0% to population x 40%</t>
-  </si>
-  <si>
-    <t>2022-2032 varying the CD quantifer from population x 0% to population x 50%</t>
+    <t>Only in years between campaigns, varying the CD quantifier from population x 0% to population x 40%</t>
+  </si>
+  <si>
+    <t>2022-2032 varying the CD quantifier from population x 0% to population x 50%</t>
+  </si>
+  <si>
+    <t>Number of different iterations per scenario</t>
+  </si>
+  <si>
+    <t>In 2022, 2025, 2028, 2031, 2034, varying from population / 0.1-2.0</t>
+  </si>
+  <si>
+    <t>In 2022, 2024, 2026, 2028, 2030, 2032, 2034 varying from population / 0.5-2.0</t>
   </si>
 </sst>
 </file>
@@ -598,7 +604,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -654,7 +660,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>51</v>
@@ -671,7 +677,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>41</v>
@@ -682,7 +688,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -691,7 +697,7 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="79" customHeight="1" x14ac:dyDescent="0.2">
@@ -699,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
@@ -708,16 +714,16 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <f>SUM(E2:E6)</f>
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change "iterations" to "models"
</commit_message>
<xml_diff>
--- a/data/scenario_table_text.xlsx
+++ b/data/scenario_table_text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahkoenker/Dropbox/R Directory/Quantification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDF94B5-AB8D-DD4F-A36D-E89C01183B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C21D18-ED2A-164B-BD39-A1B8F179E375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D175AB0F-402B-D841-A3E2-CFF385259FBB}"/>
   </bookViews>
@@ -105,22 +105,22 @@
     <t>2020-2035 using population x 6%</t>
   </si>
   <si>
-    <t>Total iterations</t>
-  </si>
-  <si>
     <t>Only in years between campaigns, varying the CD quantifier from population x 0% to population x 40%</t>
   </si>
   <si>
     <t>2022-2032 varying the CD quantifier from population x 0% to population x 50%</t>
   </si>
   <si>
-    <t>Number of different iterations per scenario</t>
-  </si>
-  <si>
     <t>In 2022, 2025, 2028, 2031, 2034, varying from population / 0.1-2.0</t>
   </si>
   <si>
     <t>In 2022, 2024, 2026, 2028, 2030, 2032, 2034 varying from population / 0.5-2.0</t>
+  </si>
+  <si>
+    <t>Number of different models per scenario</t>
+  </si>
+  <si>
+    <t>Total models</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>51</v>
@@ -677,7 +677,7 @@
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>41</v>
@@ -688,7 +688,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -705,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <f>SUM(E2:E6)</f>

</xml_diff>